<commit_message>
Se reparan los test cases, todo funcional  y agregado
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Correo</t>
   </si>
@@ -55,6 +55,39 @@
   </si>
   <si>
     <t>calle falsa 123</t>
+  </si>
+  <si>
+    <t>Pais</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Antioquia</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>Medellin</t>
+  </si>
+  <si>
+    <t>NumTel</t>
+  </si>
+  <si>
+    <t>TipoID</t>
+  </si>
+  <si>
+    <t>NumID</t>
+  </si>
+  <si>
+    <t>Cédula de Ciudadanía</t>
+  </si>
+  <si>
+    <t>123456789</t>
   </si>
 </sst>
 </file>
@@ -90,9 +123,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,34 +444,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="9" width="11.42578125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>